<commit_message>
updates to blossom strategy
</commit_message>
<xml_diff>
--- a/anther/src/main/resources/documentation/Backtesting.xlsx
+++ b/anther/src/main/resources/documentation/Backtesting.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPrizio\IdeaProjects\bluebell\anther\src\main\resources\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\IdeaProjects\bluebell\anther\src\main\resources\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38247FAD-3C69-498F-AE5F-516459F6C1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5763C2CC-521F-4F6E-B5D7-9382C5F0240C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E258FCD5-B2C9-43D2-863F-B9659CD81F11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{E258FCD5-B2C9-43D2-863F-B9659CD81F11}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="7" r:id="rId1"/>
     <sheet name="Bloom (Expanded)" sheetId="10" r:id="rId2"/>
     <sheet name="Bloom Review" sheetId="11" r:id="rId3"/>
+    <sheet name="Bloom 2.0" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="47">
   <si>
     <t>2024 with 30 point normalization</t>
   </si>
@@ -119,6 +120,66 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>Buy TP</t>
+  </si>
+  <si>
+    <t>Buy SL</t>
+  </si>
+  <si>
+    <t>Sell TP</t>
+  </si>
+  <si>
+    <t>Sell SL</t>
+  </si>
+  <si>
+    <t>Win %</t>
+  </si>
+  <si>
+    <t>Profitability</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Max Drawdown</t>
+  </si>
+  <si>
+    <t>Abs. Drawdown</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>Lot Size: 0.4</t>
+  </si>
+  <si>
+    <t>Max Size: 0.56</t>
+  </si>
+  <si>
+    <t>Hour: 15</t>
+  </si>
+  <si>
+    <t>Hour: 11</t>
+  </si>
+  <si>
+    <t>Hour: 14</t>
   </si>
 </sst>
 </file>
@@ -218,7 +279,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,15 +332,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -287,16 +339,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -657,55 +721,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="21">
+      <c r="A1" s="28">
         <v>2024</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="20">
+      <c r="B1" s="28"/>
+      <c r="C1" s="26">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D1" s="20">
+      <c r="D1" s="26">
         <v>0.39930555555555558</v>
       </c>
-      <c r="E1" s="20">
+      <c r="E1" s="26">
         <v>0.40277777777777801</v>
       </c>
-      <c r="F1" s="20">
+      <c r="F1" s="26">
         <v>0.40625</v>
       </c>
-      <c r="G1" s="20">
+      <c r="G1" s="26">
         <v>0.40972222222222199</v>
       </c>
-      <c r="H1" s="20">
+      <c r="H1" s="26">
         <v>0.41319444444444497</v>
       </c>
-      <c r="I1" s="20">
+      <c r="I1" s="26">
         <v>0.41666666666666702</v>
       </c>
       <c r="J1" s="10"/>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="20">
+      <c r="M1" s="27"/>
+      <c r="N1" s="26">
         <v>0.39583333333333331</v>
       </c>
-      <c r="O1" s="20">
+      <c r="O1" s="26">
         <v>0.39930555555555558</v>
       </c>
-      <c r="P1" s="20">
+      <c r="P1" s="26">
         <v>0.40277777777777801</v>
       </c>
-      <c r="Q1" s="20">
+      <c r="Q1" s="26">
         <v>0.40625</v>
       </c>
-      <c r="R1" s="20">
+      <c r="R1" s="26">
         <v>0.40972222222222199</v>
       </c>
-      <c r="S1" s="20">
+      <c r="S1" s="26">
         <v>0.41319444444444497</v>
       </c>
-      <c r="T1" s="20">
+      <c r="T1" s="26">
         <v>0.41666666666666702</v>
       </c>
       <c r="U1" s="1"/>
@@ -714,25 +778,25 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
       <c r="J2" s="10"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
       <c r="U2" s="1"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3" t="s">
@@ -752,10 +816,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="25">
         <v>0</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="2">
         <v>104.08</v>
       </c>
@@ -778,10 +842,10 @@
         <v>113.01</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="L3" s="19">
+      <c r="L3" s="25">
         <v>0</v>
       </c>
-      <c r="M3" s="19"/>
+      <c r="M3" s="25"/>
       <c r="N3" s="2">
         <v>-119.26</v>
       </c>
@@ -824,8 +888,8 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="7">
         <f xml:space="preserve"> PRODUCT(C3,$W1)</f>
         <v>993.96400000000006</v>
@@ -855,8 +919,8 @@
         <v>1079.2455000000002</v>
       </c>
       <c r="J4" s="11"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
       <c r="N4" s="7">
         <f xml:space="preserve"> PRODUCT(N3,$W1)</f>
         <v>-1138.9330000000002</v>
@@ -906,8 +970,8 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="5">
         <v>0.68</v>
       </c>
@@ -933,8 +997,8 @@
         <f>AVERAGE(C5:I5)</f>
         <v>0.69142857142857139</v>
       </c>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
       <c r="N5" s="5">
         <v>0.61</v>
       </c>
@@ -1002,10 +1066,10 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="25">
         <v>0.05</v>
       </c>
-      <c r="B7" s="19"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="2">
         <v>-54.64</v>
       </c>
@@ -1028,10 +1092,10 @@
         <v>362.79</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="L7" s="19">
+      <c r="L7" s="25">
         <v>0.05</v>
       </c>
-      <c r="M7" s="19"/>
+      <c r="M7" s="25"/>
       <c r="N7" s="2">
         <v>205.86</v>
       </c>
@@ -1074,8 +1138,8 @@
       </c>
     </row>
     <row r="8" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="7">
         <f xml:space="preserve"> PRODUCT(C7,$W1)</f>
         <v>-521.81200000000001</v>
@@ -1105,8 +1169,8 @@
         <v>3464.6445000000003</v>
       </c>
       <c r="J8" s="11"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
       <c r="N8" s="7">
         <f xml:space="preserve"> PRODUCT(N7,$W1)</f>
         <v>1965.9630000000002</v>
@@ -1156,8 +1220,8 @@
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="5">
         <v>0.66</v>
       </c>
@@ -1183,8 +1247,8 @@
         <f>AVERAGE(C9:I9)</f>
         <v>0.69142857142857139</v>
       </c>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
       <c r="N9" s="6">
         <v>0.64</v>
       </c>
@@ -1259,10 +1323,10 @@
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="A11" s="25">
         <v>0.1</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="2">
         <v>28.62</v>
       </c>
@@ -1285,10 +1349,10 @@
         <v>502.63</v>
       </c>
       <c r="J11" s="1"/>
-      <c r="L11" s="19">
+      <c r="L11" s="25">
         <v>0.1</v>
       </c>
-      <c r="M11" s="19"/>
+      <c r="M11" s="25"/>
       <c r="N11" s="2">
         <v>42.3</v>
       </c>
@@ -1331,8 +1395,8 @@
       </c>
     </row>
     <row r="12" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="7">
         <f xml:space="preserve"> PRODUCT(C11,$W1)</f>
         <v>273.32100000000003</v>
@@ -1362,8 +1426,8 @@
         <v>4800.1165000000001</v>
       </c>
       <c r="J12" s="11"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
       <c r="N12" s="7">
         <f xml:space="preserve"> PRODUCT(N11,$W1)</f>
         <v>403.96499999999997</v>
@@ -1413,8 +1477,8 @@
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="5">
         <v>0.67</v>
       </c>
@@ -1440,8 +1504,8 @@
         <f>AVERAGE(C13:I13)</f>
         <v>0.68571428571428572</v>
       </c>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
       <c r="N13" s="6">
         <v>0.62</v>
       </c>
@@ -1516,10 +1580,10 @@
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="25">
         <v>0.15</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="2">
         <v>-1.73</v>
       </c>
@@ -1542,10 +1606,10 @@
         <v>254.89</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="L15" s="19">
+      <c r="L15" s="25">
         <v>0.15</v>
       </c>
-      <c r="M15" s="19"/>
+      <c r="M15" s="25"/>
       <c r="N15" s="2">
         <v>101.65</v>
       </c>
@@ -1570,8 +1634,8 @@
       <c r="U15" s="1"/>
     </row>
     <row r="16" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="7">
         <f xml:space="preserve"> PRODUCT(C15,$W1)</f>
         <v>-16.5215</v>
@@ -1601,8 +1665,8 @@
         <v>2434.1995000000002</v>
       </c>
       <c r="J16" s="11"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
       <c r="N16" s="7">
         <f xml:space="preserve"> PRODUCT(N15,$W1)</f>
         <v>970.75750000000016</v>
@@ -1640,8 +1704,8 @@
       <c r="AC16" s="13"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="5">
         <v>0.66</v>
       </c>
@@ -1667,8 +1731,8 @@
         <f>AVERAGE(C17:I17)</f>
         <v>0.68142857142857138</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
       <c r="N17" s="6">
         <v>0.63</v>
       </c>
@@ -1707,10 +1771,10 @@
       <c r="U18" s="1"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="25">
         <v>0.2</v>
       </c>
-      <c r="B19" s="19"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="2">
         <v>90.64</v>
       </c>
@@ -1733,10 +1797,10 @@
         <v>76.650000000000006</v>
       </c>
       <c r="J19" s="1"/>
-      <c r="L19" s="19">
+      <c r="L19" s="25">
         <v>0.2</v>
       </c>
-      <c r="M19" s="19"/>
+      <c r="M19" s="25"/>
       <c r="N19" s="2">
         <v>294.07</v>
       </c>
@@ -1761,8 +1825,8 @@
       <c r="U19" s="1"/>
     </row>
     <row r="20" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="7">
         <f xml:space="preserve"> PRODUCT(C19,$W1)</f>
         <v>865.61200000000008</v>
@@ -1792,8 +1856,8 @@
         <v>732.00750000000016</v>
       </c>
       <c r="J20" s="11"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
       <c r="N20" s="7">
         <f xml:space="preserve"> PRODUCT(N19, $W1)</f>
         <v>2808.3685</v>
@@ -1831,8 +1895,8 @@
       <c r="AC20" s="13"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="5">
         <v>0.67</v>
       </c>
@@ -1858,8 +1922,8 @@
         <f>AVERAGE(C21:I21)</f>
         <v>0.68428571428571427</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
       <c r="N21" s="6">
         <v>0.65</v>
       </c>
@@ -1898,10 +1962,10 @@
       <c r="U22" s="1"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
+      <c r="A23" s="25">
         <v>0.25</v>
       </c>
-      <c r="B23" s="19"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="2">
         <v>110.5</v>
       </c>
@@ -1924,10 +1988,10 @@
         <v>77.95</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="L23" s="19">
+      <c r="L23" s="25">
         <v>0.25</v>
       </c>
-      <c r="M23" s="19"/>
+      <c r="M23" s="25"/>
       <c r="N23" s="2">
         <v>420.99</v>
       </c>
@@ -1952,8 +2016,8 @@
       <c r="U23" s="1"/>
     </row>
     <row r="24" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="7">
         <f xml:space="preserve"> PRODUCT(C23,$W1)</f>
         <v>1055.2750000000001</v>
@@ -1983,8 +2047,8 @@
         <v>744.42250000000013</v>
       </c>
       <c r="J24" s="11"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
       <c r="N24" s="7">
         <f>PRODUCT(N23, $W1)</f>
         <v>4020.4545000000003</v>
@@ -2022,8 +2086,8 @@
       <c r="AC24" s="13"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="5">
         <v>0.67</v>
       </c>
@@ -2049,8 +2113,8 @@
         <f>AVERAGE(C25:I25)</f>
         <v>0.68285714285714272</v>
       </c>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
       <c r="N25" s="6">
         <v>0.65</v>
       </c>
@@ -2079,20 +2143,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="L11:M13"/>
-    <mergeCell ref="L15:M17"/>
-    <mergeCell ref="L19:M21"/>
-    <mergeCell ref="L23:M25"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="L3:M5"/>
-    <mergeCell ref="L7:M9"/>
-    <mergeCell ref="L1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="A23:B25"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
@@ -2107,6 +2157,20 @@
     <mergeCell ref="A11:B13"/>
     <mergeCell ref="A15:B17"/>
     <mergeCell ref="A19:B21"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="L3:M5"/>
+    <mergeCell ref="L7:M9"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="L11:M13"/>
+    <mergeCell ref="L15:M17"/>
+    <mergeCell ref="L19:M21"/>
+    <mergeCell ref="L23:M25"/>
+    <mergeCell ref="R1:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2170,7 +2234,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="A2" s="28">
         <v>2020</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2222,7 +2286,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2268,7 +2332,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="28">
         <v>2021</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2320,7 +2384,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2366,7 +2430,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+      <c r="A6" s="28">
         <v>2022</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2418,7 +2482,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2464,7 +2528,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="28">
         <v>2023</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2516,7 +2580,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2562,7 +2626,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="28">
         <v>2024</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2614,7 +2678,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2761,7 +2825,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="28">
         <v>2020</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2813,7 +2877,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
@@ -2859,7 +2923,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="28">
         <v>2021</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2911,7 +2975,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2957,7 +3021,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="28">
         <v>2022</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -3009,7 +3073,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
@@ -3055,7 +3119,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="28">
         <v>2023</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3107,7 +3171,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
@@ -3153,7 +3217,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23" s="28">
         <v>2024</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -3205,7 +3269,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
@@ -3328,16 +3392,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3348,2312 +3412,2312 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36D5E42-3CD6-4286-BF6E-C293A0AE05C2}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="24">
+      <c r="B1" s="21">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C1" s="24">
+      <c r="C1" s="21">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D1" s="24">
+      <c r="D1" s="21">
         <v>0.40277777777777801</v>
       </c>
-      <c r="E1" s="24">
+      <c r="E1" s="21">
         <v>0.40625</v>
       </c>
-      <c r="F1" s="24">
+      <c r="F1" s="21">
         <v>0.40972222222222199</v>
       </c>
-      <c r="G1" s="24">
+      <c r="G1" s="21">
         <v>0.41319444444444497</v>
       </c>
-      <c r="H1" s="24">
+      <c r="H1" s="21">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="24">
+      <c r="K1" s="21">
         <v>0.39583333333333331</v>
       </c>
-      <c r="L1" s="24">
+      <c r="L1" s="21">
         <v>0.39930555555555558</v>
       </c>
-      <c r="M1" s="24">
+      <c r="M1" s="21">
         <v>0.40277777777777801</v>
       </c>
-      <c r="N1" s="24">
+      <c r="N1" s="21">
         <v>0.40625</v>
       </c>
-      <c r="O1" s="24">
+      <c r="O1" s="21">
         <v>0.40972222222222199</v>
       </c>
-      <c r="P1" s="24">
+      <c r="P1" s="21">
         <v>0.41319444444444497</v>
       </c>
-      <c r="Q1" s="24">
+      <c r="Q1" s="21">
         <v>0.41666666666666702</v>
       </c>
-      <c r="R1" s="23"/>
+      <c r="R1" s="20"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="29">
         <v>2020</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="26">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="29">
         <v>2020</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="23"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="20"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
+      <c r="A3" s="23">
         <v>0</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="20">
         <v>470.19</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="20">
         <v>733.19</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="20">
         <v>467.03</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="20">
         <v>539.82000000000005</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="20">
         <v>-202.09</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="20">
         <v>1547.13</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="20">
         <v>794.83</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="27">
+      <c r="I3" s="20"/>
+      <c r="J3" s="23">
         <v>0</v>
       </c>
-      <c r="K3" s="28">
+      <c r="K3" s="20">
         <v>1024.1300000000001</v>
       </c>
-      <c r="L3" s="28">
+      <c r="L3" s="20">
         <v>369.88</v>
       </c>
-      <c r="M3" s="28">
+      <c r="M3" s="20">
         <v>242.69</v>
       </c>
-      <c r="N3" s="28">
+      <c r="N3" s="20">
         <v>162.07</v>
       </c>
-      <c r="O3" s="28">
+      <c r="O3" s="20">
         <v>-11.83</v>
       </c>
-      <c r="P3" s="28">
+      <c r="P3" s="20">
         <v>1491.66</v>
       </c>
-      <c r="Q3" s="28">
+      <c r="Q3" s="20">
         <v>700.98</v>
       </c>
-      <c r="R3" s="23"/>
+      <c r="R3" s="20"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
+      <c r="A4" s="23">
         <v>0.05</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="20">
         <v>747.45</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="20">
         <v>560.64</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="20">
         <v>244.89</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="20">
         <v>570.48</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="20">
         <v>-236.21</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="20">
         <v>1708.82</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="20">
         <v>450.05</v>
       </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="27">
+      <c r="I4" s="20"/>
+      <c r="J4" s="23">
         <v>0.05</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="20">
         <v>1069.95</v>
       </c>
-      <c r="L4" s="28">
+      <c r="L4" s="20">
         <v>202.38</v>
       </c>
-      <c r="M4" s="28">
+      <c r="M4" s="20">
         <v>301.56</v>
       </c>
-      <c r="N4" s="28">
+      <c r="N4" s="20">
         <v>-50.01</v>
       </c>
-      <c r="O4" s="28">
+      <c r="O4" s="20">
         <v>-78.13</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="20">
         <v>1154.32</v>
       </c>
-      <c r="Q4" s="28">
+      <c r="Q4" s="20">
         <v>214.9</v>
       </c>
-      <c r="R4" s="23"/>
+      <c r="R4" s="20"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+      <c r="A5" s="23">
         <v>0.1</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="20">
         <v>838</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="20">
         <v>396.02</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="20">
         <v>261.88</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="20">
         <v>70.19</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="20">
         <v>-172.91</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="20">
         <v>1189.69</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="20">
         <v>519.63</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="27">
+      <c r="I5" s="20"/>
+      <c r="J5" s="23">
         <v>0.1</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="20">
         <v>946.31</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="20">
         <v>289.66000000000003</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="20">
         <v>232.35</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="20">
         <v>-238.88</v>
       </c>
-      <c r="O5" s="28">
+      <c r="O5" s="20">
         <v>-33.020000000000003</v>
       </c>
-      <c r="P5" s="28">
+      <c r="P5" s="20">
         <v>1168.0999999999999</v>
       </c>
-      <c r="Q5" s="28">
+      <c r="Q5" s="20">
         <v>73.040000000000006</v>
       </c>
-      <c r="R5" s="23"/>
+      <c r="R5" s="20"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
+      <c r="A6" s="23">
         <v>0.15</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="20">
         <v>1176.6099999999999</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="20">
         <v>350.12</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="20">
         <v>114.12</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="20">
         <v>-198.55</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="20">
         <v>176.81</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="20">
         <v>1342.46</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="20">
         <v>749.07</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="27">
+      <c r="I6" s="20"/>
+      <c r="J6" s="23">
         <v>0.15</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="20">
         <v>1037.53</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="20">
         <v>477.34</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M6" s="20">
         <v>-407.51</v>
       </c>
-      <c r="N6" s="28">
+      <c r="N6" s="20">
         <v>-361</v>
       </c>
-      <c r="O6" s="28">
+      <c r="O6" s="20">
         <v>334.41</v>
       </c>
-      <c r="P6" s="28">
+      <c r="P6" s="20">
         <v>1116.06</v>
       </c>
-      <c r="Q6" s="28">
+      <c r="Q6" s="20">
         <v>182.51</v>
       </c>
-      <c r="R6" s="23"/>
+      <c r="R6" s="20"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="27">
+      <c r="A7" s="23">
         <v>0.2</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="20">
         <v>906.45</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="20">
         <v>344.15</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="20">
         <v>106.59</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="20">
         <v>-678.8</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="20">
         <v>289.26</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="20">
         <v>990.6</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="20">
         <v>458.21</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="27">
+      <c r="I7" s="20"/>
+      <c r="J7" s="23">
         <v>0.2</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="20">
         <v>1120.73</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="20">
         <v>724.21</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7" s="20">
         <v>-460.68</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="20">
         <v>-479.42</v>
       </c>
-      <c r="O7" s="28">
+      <c r="O7" s="20">
         <v>366.52</v>
       </c>
-      <c r="P7" s="28">
+      <c r="P7" s="20">
         <v>1339.02</v>
       </c>
-      <c r="Q7" s="28">
+      <c r="Q7" s="20">
         <v>347.4</v>
       </c>
-      <c r="R7" s="23"/>
+      <c r="R7" s="20"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+      <c r="A8" s="23">
         <v>0.25</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="20">
         <v>1000.99</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="20">
         <v>268.08</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="20">
         <v>-51.11</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="20">
         <v>-391.34</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="20">
         <v>562.72</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="20">
         <v>1255.1099999999999</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="20">
         <v>303.5</v>
       </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="27">
+      <c r="I8" s="20"/>
+      <c r="J8" s="23">
         <v>0.25</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="20">
         <v>851.7</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="20">
         <v>186.83</v>
       </c>
-      <c r="M8" s="28">
+      <c r="M8" s="20">
         <v>-724.43</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="20">
         <v>-486.51</v>
       </c>
-      <c r="O8" s="28">
+      <c r="O8" s="20">
         <v>598.27</v>
       </c>
-      <c r="P8" s="28">
+      <c r="P8" s="20">
         <v>1523.83</v>
       </c>
-      <c r="Q8" s="28">
+      <c r="Q8" s="20">
         <v>376.01</v>
       </c>
-      <c r="R8" s="23"/>
+      <c r="R8" s="20"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="26">
+      <c r="A9" s="29">
         <v>2021</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="26">
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="29">
         <v>2021</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="23"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="20"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
+      <c r="A10" s="23">
         <v>0</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="20">
         <v>620.41</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="20">
         <v>978</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>-5.89</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="20">
         <v>85.33</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>1170.17</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>860.11</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="20">
         <v>97.93</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="27">
+      <c r="I10" s="20"/>
+      <c r="J10" s="23">
         <v>0</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="20">
         <v>478.01</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="20">
         <v>1253.75</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10" s="20">
         <v>243.08</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="20">
         <v>617.34</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="20">
         <v>1492.79</v>
       </c>
-      <c r="P10" s="23">
+      <c r="P10" s="20">
         <v>1457.12</v>
       </c>
-      <c r="Q10" s="23">
+      <c r="Q10" s="20">
         <v>286.44</v>
       </c>
-      <c r="R10" s="23"/>
+      <c r="R10" s="20"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
+      <c r="A11" s="23">
         <v>0.05</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="20">
         <v>361.11</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="20">
         <v>942.33</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="20">
         <v>-247.33</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="20">
         <v>302.20999999999998</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="20">
         <v>1046.69</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>957.28</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="20">
         <v>147.24</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="27">
+      <c r="I11" s="20"/>
+      <c r="J11" s="23">
         <v>0.05</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="20">
         <v>404.17</v>
       </c>
-      <c r="L11" s="23">
+      <c r="L11" s="20">
         <v>1280.56</v>
       </c>
-      <c r="M11" s="23">
+      <c r="M11" s="20">
         <v>126.79</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="20">
         <v>618.59</v>
       </c>
-      <c r="O11" s="23">
+      <c r="O11" s="20">
         <v>1652.63</v>
       </c>
-      <c r="P11" s="23">
+      <c r="P11" s="20">
         <v>1460.79</v>
       </c>
-      <c r="Q11" s="23">
+      <c r="Q11" s="20">
         <v>474.33</v>
       </c>
-      <c r="R11" s="23"/>
+      <c r="R11" s="20"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+      <c r="A12" s="23">
         <v>0.1</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="20">
         <v>361.78</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>1138.49</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>-250.05</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="20">
         <v>282.11</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>975.69</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>1069.6300000000001</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="20">
         <v>209.44</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="27">
+      <c r="I12" s="20"/>
+      <c r="J12" s="23">
         <v>0.1</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="20">
         <v>486.04</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="20">
         <v>1551.68</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="20">
         <v>394.19</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="20">
         <v>694.27</v>
       </c>
-      <c r="O12" s="23">
+      <c r="O12" s="20">
         <v>1632.29</v>
       </c>
-      <c r="P12" s="23">
+      <c r="P12" s="20">
         <v>1370.48</v>
       </c>
-      <c r="Q12" s="23">
+      <c r="Q12" s="20">
         <v>570.92999999999995</v>
       </c>
-      <c r="R12" s="23"/>
+      <c r="R12" s="20"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
+      <c r="A13" s="23">
         <v>0.15</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="20">
         <v>365.17</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="20">
         <v>1265.8699999999999</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="20">
         <v>-161.63999999999999</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="20">
         <v>572.39</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="20">
         <v>1229.4000000000001</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <v>788.48</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="20">
         <v>240.33</v>
       </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="27">
+      <c r="I13" s="20"/>
+      <c r="J13" s="23">
         <v>0.15</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="20">
         <v>321.47000000000003</v>
       </c>
-      <c r="L13" s="23">
+      <c r="L13" s="20">
         <v>1490.42</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M13" s="20">
         <v>705.73</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="20">
         <v>760.5</v>
       </c>
-      <c r="O13" s="23">
+      <c r="O13" s="20">
         <v>1934.67</v>
       </c>
-      <c r="P13" s="23">
+      <c r="P13" s="20">
         <v>1022.76</v>
       </c>
-      <c r="Q13" s="23">
+      <c r="Q13" s="20">
         <v>783.11</v>
       </c>
-      <c r="R13" s="23"/>
+      <c r="R13" s="20"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
+      <c r="A14" s="23">
         <v>0.2</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="20">
         <v>375.24</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="20">
         <v>1318.44</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="20">
         <v>-34.92</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="20">
         <v>1027.22</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>1246.9100000000001</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <v>929.45</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="20">
         <v>503.53</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="27">
+      <c r="I14" s="20"/>
+      <c r="J14" s="23">
         <v>0.2</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="20">
         <v>0.86</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="20">
         <v>1523.82</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="20">
         <v>921.42</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="20">
         <v>610.75</v>
       </c>
-      <c r="O14" s="23">
+      <c r="O14" s="20">
         <v>1848.99</v>
       </c>
-      <c r="P14" s="23">
+      <c r="P14" s="20">
         <v>1339.53</v>
       </c>
-      <c r="Q14" s="23">
+      <c r="Q14" s="20">
         <v>929.12</v>
       </c>
-      <c r="R14" s="23"/>
+      <c r="R14" s="20"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
+      <c r="A15" s="23">
         <v>0.25</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="20">
         <v>226.01</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="20">
         <v>1586.27</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="20">
         <v>203.97</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="20">
         <v>1205.27</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="20">
         <v>1152.17</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="20">
         <v>1257.74</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="20">
         <v>406.74</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="27">
+      <c r="I15" s="20"/>
+      <c r="J15" s="23">
         <v>0.25</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="20">
         <v>-260.25</v>
       </c>
-      <c r="L15" s="23">
+      <c r="L15" s="20">
         <v>1751.54</v>
       </c>
-      <c r="M15" s="23">
+      <c r="M15" s="20">
         <v>1108.74</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="20">
         <v>1080.1500000000001</v>
       </c>
-      <c r="O15" s="23">
+      <c r="O15" s="20">
         <v>1903.44</v>
       </c>
-      <c r="P15" s="23">
+      <c r="P15" s="20">
         <v>1640.42</v>
       </c>
-      <c r="Q15" s="23">
+      <c r="Q15" s="20">
         <v>933.17</v>
       </c>
-      <c r="R15" s="23"/>
+      <c r="R15" s="20"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="26">
+      <c r="A16" s="29">
         <v>2022</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="26">
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="29">
         <v>2022</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="23"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="20"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="27">
+      <c r="A17" s="23">
         <v>0</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="20">
         <v>701.86</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="20">
         <v>807.39</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="20">
         <v>1968.22</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="20">
         <v>596.33000000000004</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="20">
         <v>701.86</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="20">
         <v>174.21</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="20">
         <v>658.66</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="27">
+      <c r="I17" s="20"/>
+      <c r="J17" s="23">
         <v>0</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="20">
         <v>1155.49</v>
       </c>
-      <c r="L17" s="23">
+      <c r="L17" s="20">
         <v>960.99</v>
       </c>
-      <c r="M17" s="23">
+      <c r="M17" s="20">
         <v>2585.34</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="20">
         <v>816.17</v>
       </c>
-      <c r="O17" s="23">
+      <c r="O17" s="20">
         <v>783.05</v>
       </c>
-      <c r="P17" s="23">
+      <c r="P17" s="20">
         <v>458.18</v>
       </c>
-      <c r="Q17" s="23">
+      <c r="Q17" s="20">
         <v>549.41</v>
       </c>
-      <c r="R17" s="23"/>
+      <c r="R17" s="20"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="27">
+      <c r="A18" s="23">
         <v>0.05</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="20">
         <v>1401.92</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="20">
         <v>626.25</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="20">
         <v>2288.4</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="20">
         <v>1180.3</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="20">
         <v>958.68</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="20">
         <v>72.2</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="20">
         <v>1133.58</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="27">
+      <c r="I18" s="20"/>
+      <c r="J18" s="23">
         <v>0.05</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="20">
         <v>1350.51</v>
       </c>
-      <c r="L18" s="23">
+      <c r="L18" s="20">
         <v>583.57000000000005</v>
       </c>
-      <c r="M18" s="23">
+      <c r="M18" s="20">
         <v>2817.06</v>
       </c>
-      <c r="N18" s="23">
+      <c r="N18" s="20">
         <v>1283.18</v>
       </c>
-      <c r="O18" s="23">
+      <c r="O18" s="20">
         <v>942.07</v>
       </c>
-      <c r="P18" s="23">
+      <c r="P18" s="20">
         <v>200.79</v>
       </c>
-      <c r="Q18" s="23">
+      <c r="Q18" s="20">
         <v>882.58</v>
       </c>
-      <c r="R18" s="23"/>
+      <c r="R18" s="20"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="27">
+      <c r="A19" s="23">
         <v>0.1</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="20">
         <v>1350.92</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="20">
         <v>756.99</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="20">
         <v>2395.64</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="20">
         <v>1350.92</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="20">
         <v>654.44000000000005</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="20">
         <v>660.79</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="20">
         <v>1068.53</v>
       </c>
-      <c r="I19" s="23"/>
-      <c r="J19" s="27">
+      <c r="I19" s="20"/>
+      <c r="J19" s="23">
         <v>0.1</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K19" s="20">
         <v>1074.42</v>
       </c>
-      <c r="L19" s="23">
+      <c r="L19" s="20">
         <v>926.59</v>
       </c>
-      <c r="M19" s="23">
+      <c r="M19" s="20">
         <v>2378.67</v>
       </c>
-      <c r="N19" s="23">
+      <c r="N19" s="20">
         <v>771.69</v>
       </c>
-      <c r="O19" s="23">
+      <c r="O19" s="20">
         <v>985.65</v>
       </c>
-      <c r="P19" s="23">
+      <c r="P19" s="20">
         <v>301.54000000000002</v>
       </c>
-      <c r="Q19" s="23">
+      <c r="Q19" s="20">
         <v>1176.74</v>
       </c>
-      <c r="R19" s="23"/>
+      <c r="R19" s="20"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="27">
+      <c r="A20" s="23">
         <v>0.15</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="20">
         <v>805.72</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="20">
         <v>788.67</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="20">
         <v>1881.99</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="20">
         <v>1048.44</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="20">
         <v>927.08</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="20">
         <v>927.84</v>
       </c>
-      <c r="H20" s="23">
+      <c r="H20" s="20">
         <v>1690.68</v>
       </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="27">
+      <c r="I20" s="20"/>
+      <c r="J20" s="23">
         <v>0.15</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="20">
         <v>861.9</v>
       </c>
-      <c r="L20" s="23">
+      <c r="L20" s="20">
         <v>537.89</v>
       </c>
-      <c r="M20" s="23">
+      <c r="M20" s="20">
         <v>1520.27</v>
       </c>
-      <c r="N20" s="23">
+      <c r="N20" s="20">
         <v>788.14</v>
       </c>
-      <c r="O20" s="23">
+      <c r="O20" s="20">
         <v>806.48</v>
       </c>
-      <c r="P20" s="23">
+      <c r="P20" s="20">
         <v>443.81</v>
       </c>
-      <c r="Q20" s="23">
+      <c r="Q20" s="20">
         <v>1620.46</v>
       </c>
-      <c r="R20" s="23"/>
+      <c r="R20" s="20"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
+      <c r="A21" s="23">
         <v>0.2</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="20">
         <v>840.92</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="20">
         <v>567.07000000000005</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="20">
         <v>1834.55</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="20">
         <v>714.28</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="20">
         <v>1347.48</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="20">
         <v>1601.95</v>
       </c>
-      <c r="H21" s="23">
+      <c r="H21" s="20">
         <v>1658.61</v>
       </c>
-      <c r="I21" s="23"/>
-      <c r="J21" s="27">
+      <c r="I21" s="20"/>
+      <c r="J21" s="23">
         <v>0.2</v>
       </c>
-      <c r="K21" s="23">
+      <c r="K21" s="20">
         <v>763.96</v>
       </c>
-      <c r="L21" s="23">
+      <c r="L21" s="20">
         <v>1279.77</v>
       </c>
-      <c r="M21" s="23">
+      <c r="M21" s="20">
         <v>1564.43</v>
       </c>
-      <c r="N21" s="23">
+      <c r="N21" s="20">
         <v>416.85</v>
       </c>
-      <c r="O21" s="23">
+      <c r="O21" s="20">
         <v>606.36</v>
       </c>
-      <c r="P21" s="23">
+      <c r="P21" s="20">
         <v>600.55999999999995</v>
       </c>
-      <c r="Q21" s="23">
+      <c r="Q21" s="20">
         <v>1729.1</v>
       </c>
-      <c r="R21" s="23"/>
+      <c r="R21" s="20"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
+      <c r="A22" s="23">
         <v>0.25</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="20">
         <v>1139.96</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="20">
         <v>852.03</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="20">
         <v>1168.02</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="20">
         <v>450.69</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="20">
         <v>881.58</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="20">
         <v>1663.55</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="20">
         <v>1748.46</v>
       </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="27">
+      <c r="I22" s="20"/>
+      <c r="J22" s="23">
         <v>0.25</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="20">
         <v>672.95</v>
       </c>
-      <c r="L22" s="23">
+      <c r="L22" s="20">
         <v>964.46</v>
       </c>
-      <c r="M22" s="23">
+      <c r="M22" s="20">
         <v>1587.95</v>
       </c>
-      <c r="N22" s="23">
+      <c r="N22" s="20">
         <v>170.46</v>
       </c>
-      <c r="O22" s="23">
+      <c r="O22" s="20">
         <v>586.07000000000005</v>
       </c>
-      <c r="P22" s="23">
+      <c r="P22" s="20">
         <v>881.14</v>
       </c>
-      <c r="Q22" s="23">
+      <c r="Q22" s="20">
         <v>2170.75</v>
       </c>
-      <c r="R22" s="23"/>
+      <c r="R22" s="20"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="26">
+      <c r="A23" s="29">
         <v>2023</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="26">
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="29">
         <v>2023</v>
       </c>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="23"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="20"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="27">
+      <c r="A24" s="23">
         <v>0</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="20">
         <v>962.32</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="20">
         <v>-355.64</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="20">
         <v>-230.12</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="20">
         <v>836.8</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="20">
         <v>334.72</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="20">
         <v>585.76</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="20">
         <v>1150.5999999999999</v>
       </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="27">
+      <c r="I24" s="20"/>
+      <c r="J24" s="23">
         <v>0</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="20">
         <v>488.73</v>
       </c>
-      <c r="L24" s="23">
+      <c r="L24" s="20">
         <v>561.53</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="20">
         <v>276.43</v>
       </c>
-      <c r="N24" s="23">
+      <c r="N24" s="20">
         <v>875.67</v>
       </c>
-      <c r="O24" s="23">
+      <c r="O24" s="20">
         <v>718.39</v>
       </c>
-      <c r="P24" s="23">
+      <c r="P24" s="20">
         <v>956.76</v>
       </c>
-      <c r="Q24" s="23">
+      <c r="Q24" s="20">
         <v>552.5</v>
       </c>
-      <c r="R24" s="23"/>
+      <c r="R24" s="20"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="27">
+      <c r="A25" s="23">
         <v>0.05</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="20">
         <v>1008.8</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="20">
         <v>-243.3</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="20">
         <v>283.89999999999998</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="20">
         <v>877</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="20">
         <v>349.8</v>
       </c>
-      <c r="G25" s="23">
+      <c r="G25" s="20">
         <v>877</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="20">
         <v>1008.8</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="27">
+      <c r="I25" s="20"/>
+      <c r="J25" s="23">
         <v>0.05</v>
       </c>
-      <c r="K25" s="23">
+      <c r="K25" s="20">
         <v>433.96</v>
       </c>
-      <c r="L25" s="23">
+      <c r="L25" s="20">
         <v>764.68</v>
       </c>
-      <c r="M25" s="23">
+      <c r="M25" s="20">
         <v>446.5</v>
       </c>
-      <c r="N25" s="23">
+      <c r="N25" s="20">
         <v>917.58</v>
       </c>
-      <c r="O25" s="23">
+      <c r="O25" s="20">
         <v>628.98</v>
       </c>
-      <c r="P25" s="23">
+      <c r="P25" s="20">
         <v>445.68</v>
       </c>
-      <c r="Q25" s="23">
+      <c r="Q25" s="20">
         <v>709.35</v>
       </c>
-      <c r="R25" s="23"/>
+      <c r="R25" s="20"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
+      <c r="A26" s="23">
         <v>0.1</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="20">
         <v>644.28</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="20">
         <v>23.01</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="20">
         <v>575.25</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="20">
         <v>775.19</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="20">
         <v>513.15</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="20">
         <v>644.28</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="20">
         <v>989.43</v>
       </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="27">
+      <c r="I26" s="20"/>
+      <c r="J26" s="23">
         <v>0.1</v>
       </c>
-      <c r="K26" s="23">
+      <c r="K26" s="20">
         <v>-57.81</v>
       </c>
-      <c r="L26" s="23">
+      <c r="L26" s="20">
         <v>962.2</v>
       </c>
-      <c r="M26" s="23">
+      <c r="M26" s="20">
         <v>299.95</v>
       </c>
-      <c r="N26" s="23">
+      <c r="N26" s="20">
         <v>719.33</v>
       </c>
-      <c r="O26" s="23">
+      <c r="O26" s="20">
         <v>903.31</v>
       </c>
-      <c r="P26" s="23">
+      <c r="P26" s="20">
         <v>-34.090000000000003</v>
       </c>
-      <c r="Q26" s="23">
+      <c r="Q26" s="20">
         <v>437.25</v>
       </c>
-      <c r="R26" s="23"/>
+      <c r="R26" s="20"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="27">
+      <c r="A27" s="23">
         <v>0.15</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B27" s="20">
         <v>673.68</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="20">
         <v>312.77999999999997</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="20">
         <v>694.77</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="20">
         <v>758.24</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="20">
         <v>679.56</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27" s="20">
         <v>526.80999999999995</v>
       </c>
-      <c r="H27" s="23">
+      <c r="H27" s="20">
         <v>881.4</v>
       </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="27">
+      <c r="I27" s="20"/>
+      <c r="J27" s="23">
         <v>0.15</v>
       </c>
-      <c r="K27" s="23">
+      <c r="K27" s="20">
         <v>-147.84</v>
       </c>
-      <c r="L27" s="23">
+      <c r="L27" s="20">
         <v>870.58</v>
       </c>
-      <c r="M27" s="23">
+      <c r="M27" s="20">
         <v>571.79999999999995</v>
       </c>
-      <c r="N27" s="23">
+      <c r="N27" s="20">
         <v>485.78</v>
       </c>
-      <c r="O27" s="23">
+      <c r="O27" s="20">
         <v>822.34</v>
       </c>
-      <c r="P27" s="23">
+      <c r="P27" s="20">
         <v>-326.60000000000002</v>
       </c>
-      <c r="Q27" s="23">
+      <c r="Q27" s="20">
         <v>191.34</v>
       </c>
-      <c r="R27" s="23"/>
+      <c r="R27" s="20"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="27">
+      <c r="A28" s="23">
         <v>0.2</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="20">
         <v>403.32</v>
       </c>
-      <c r="C28" s="23">
+      <c r="C28" s="20">
         <v>704.56</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="20">
         <v>576.07000000000005</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="20">
         <v>791.2</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="20">
         <v>860.01</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="20">
         <v>499.21</v>
       </c>
-      <c r="H28" s="23">
+      <c r="H28" s="20">
         <v>834.65</v>
       </c>
-      <c r="I28" s="23"/>
-      <c r="J28" s="27">
+      <c r="I28" s="20"/>
+      <c r="J28" s="23">
         <v>0.2</v>
       </c>
-      <c r="K28" s="23">
+      <c r="K28" s="20">
         <v>388.84</v>
       </c>
-      <c r="L28" s="23">
+      <c r="L28" s="20">
         <v>1085.0999999999999</v>
       </c>
-      <c r="M28" s="23">
+      <c r="M28" s="20">
         <v>686.26</v>
       </c>
-      <c r="N28" s="23">
+      <c r="N28" s="20">
         <v>140.13999999999999</v>
       </c>
-      <c r="O28" s="23">
+      <c r="O28" s="20">
         <v>850.86</v>
       </c>
-      <c r="P28" s="23">
+      <c r="P28" s="20">
         <v>-434.7</v>
       </c>
-      <c r="Q28" s="23">
+      <c r="Q28" s="20">
         <v>283.68</v>
       </c>
-      <c r="R28" s="23"/>
+      <c r="R28" s="20"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
+      <c r="A29" s="23">
         <v>0.25</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="20">
         <v>431.68</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="20">
         <v>674.77</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="20">
         <v>656.52</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="20">
         <v>482.23</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="20">
         <v>536.80999999999995</v>
       </c>
-      <c r="G29" s="23">
+      <c r="G29" s="20">
         <v>594</v>
       </c>
-      <c r="H29" s="23">
+      <c r="H29" s="20">
         <v>689.32</v>
       </c>
-      <c r="I29" s="23"/>
-      <c r="J29" s="27">
+      <c r="I29" s="20"/>
+      <c r="J29" s="23">
         <v>0.25</v>
       </c>
-      <c r="K29" s="23">
+      <c r="K29" s="20">
         <v>497.66</v>
       </c>
-      <c r="L29" s="23">
+      <c r="L29" s="20">
         <v>1218.7</v>
       </c>
-      <c r="M29" s="23">
+      <c r="M29" s="20">
         <v>967.71</v>
       </c>
-      <c r="N29" s="23">
+      <c r="N29" s="20">
         <v>-181.43</v>
       </c>
-      <c r="O29" s="23">
+      <c r="O29" s="20">
         <v>650.69000000000005</v>
       </c>
-      <c r="P29" s="23">
+      <c r="P29" s="20">
         <v>295.73</v>
       </c>
-      <c r="Q29" s="23">
+      <c r="Q29" s="20">
         <v>285.14999999999998</v>
       </c>
-      <c r="R29" s="23"/>
+      <c r="R29" s="20"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="26">
+      <c r="A30" s="29">
         <v>2024</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="26">
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="29">
         <v>2024</v>
       </c>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="23"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="20"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="27">
+      <c r="A31" s="23">
         <v>0</v>
       </c>
-      <c r="B31" s="23">
+      <c r="B31" s="20">
         <v>104.08</v>
       </c>
-      <c r="C31" s="23">
+      <c r="C31" s="20">
         <v>182.14</v>
       </c>
-      <c r="D31" s="23">
+      <c r="D31" s="20">
         <v>46.18</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="20">
         <v>338.26</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="20">
         <v>316.82</v>
       </c>
-      <c r="G31" s="23">
+      <c r="G31" s="20">
         <v>307.70999999999998</v>
       </c>
-      <c r="H31" s="23">
+      <c r="H31" s="20">
         <v>113.01</v>
       </c>
-      <c r="I31" s="23"/>
-      <c r="J31" s="27">
+      <c r="I31" s="20"/>
+      <c r="J31" s="23">
         <v>0</v>
       </c>
-      <c r="K31" s="23">
+      <c r="K31" s="20">
         <v>-119.69</v>
       </c>
-      <c r="L31" s="23">
+      <c r="L31" s="20">
         <v>144.24</v>
       </c>
-      <c r="M31" s="23">
+      <c r="M31" s="20">
         <v>-23.91</v>
       </c>
-      <c r="N31" s="23">
+      <c r="N31" s="20">
         <v>274.45999999999998</v>
       </c>
-      <c r="O31" s="23">
+      <c r="O31" s="20">
         <v>474.84</v>
       </c>
-      <c r="P31" s="23">
+      <c r="P31" s="20">
         <v>637.29</v>
       </c>
-      <c r="Q31" s="23">
+      <c r="Q31" s="20">
         <v>355.03</v>
       </c>
-      <c r="R31" s="23"/>
+      <c r="R31" s="20"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="27">
+      <c r="A32" s="23">
         <v>0.05</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="20">
         <v>-54.64</v>
       </c>
-      <c r="C32" s="23">
+      <c r="C32" s="20">
         <v>27.32</v>
       </c>
-      <c r="D32" s="23">
+      <c r="D32" s="20">
         <v>-33.18</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="20">
         <v>437.12</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="20">
         <v>495.04</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="20">
         <v>322.01</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="20">
         <v>362.79</v>
       </c>
-      <c r="I32" s="23"/>
-      <c r="J32" s="27">
+      <c r="I32" s="20"/>
+      <c r="J32" s="23">
         <v>0.05</v>
       </c>
-      <c r="K32" s="23">
+      <c r="K32" s="20">
         <v>205.47</v>
       </c>
-      <c r="L32" s="23">
+      <c r="L32" s="20">
         <v>-97.03</v>
       </c>
-      <c r="M32" s="23">
+      <c r="M32" s="20">
         <v>58.02</v>
       </c>
-      <c r="N32" s="23">
+      <c r="N32" s="20">
         <v>288.24</v>
       </c>
-      <c r="O32" s="23">
+      <c r="O32" s="20">
         <v>826.08</v>
       </c>
-      <c r="P32" s="23">
+      <c r="P32" s="20">
         <v>254.28</v>
       </c>
-      <c r="Q32" s="23">
+      <c r="Q32" s="20">
         <v>453.86</v>
       </c>
-      <c r="R32" s="23"/>
+      <c r="R32" s="20"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="27">
+      <c r="A33" s="23">
         <v>0.1</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="20">
         <v>28.62</v>
       </c>
-      <c r="C33" s="23">
+      <c r="C33" s="20">
         <v>-367.43</v>
       </c>
-      <c r="D33" s="23">
+      <c r="D33" s="20">
         <v>51.38</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="20">
         <v>605.23</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="20">
         <v>502.02</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="20">
         <v>78.73</v>
       </c>
-      <c r="H33" s="23">
+      <c r="H33" s="20">
         <v>502.63</v>
       </c>
-      <c r="I33" s="23"/>
-      <c r="J33" s="27">
+      <c r="I33" s="20"/>
+      <c r="J33" s="23">
         <v>0.1</v>
       </c>
-      <c r="K33" s="23">
+      <c r="K33" s="20">
         <v>41.89</v>
       </c>
-      <c r="L33" s="23">
+      <c r="L33" s="20">
         <v>71.61</v>
       </c>
-      <c r="M33" s="23">
+      <c r="M33" s="20">
         <v>147.83000000000001</v>
       </c>
-      <c r="N33" s="23">
+      <c r="N33" s="20">
         <v>562.15</v>
       </c>
-      <c r="O33" s="23">
+      <c r="O33" s="20">
         <v>948.71</v>
       </c>
-      <c r="P33" s="23">
+      <c r="P33" s="20">
         <v>438.84</v>
       </c>
-      <c r="Q33" s="23">
+      <c r="Q33" s="20">
         <v>512.24</v>
       </c>
-      <c r="R33" s="23"/>
+      <c r="R33" s="20"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="27">
+      <c r="A34" s="23">
         <v>0.15</v>
       </c>
-      <c r="B34" s="23">
+      <c r="B34" s="20">
         <v>-1.73</v>
       </c>
-      <c r="C34" s="23">
+      <c r="C34" s="20">
         <v>-444</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D34" s="20">
         <v>144.47999999999999</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="20">
         <v>632.02</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="20">
         <v>612.05999999999995</v>
       </c>
-      <c r="G34" s="23">
+      <c r="G34" s="20">
         <v>140.01</v>
       </c>
-      <c r="H34" s="23">
+      <c r="H34" s="20">
         <v>254.89</v>
       </c>
-      <c r="I34" s="23"/>
-      <c r="J34" s="27">
+      <c r="I34" s="20"/>
+      <c r="J34" s="23">
         <v>0.15</v>
       </c>
-      <c r="K34" s="23">
+      <c r="K34" s="20">
         <v>101.24</v>
       </c>
-      <c r="L34" s="23">
+      <c r="L34" s="20">
         <v>-77.17</v>
       </c>
-      <c r="M34" s="23">
+      <c r="M34" s="20">
         <v>245.52</v>
       </c>
-      <c r="N34" s="23">
+      <c r="N34" s="20">
         <v>859.7</v>
       </c>
-      <c r="O34" s="23">
+      <c r="O34" s="20">
         <v>625.97</v>
       </c>
-      <c r="P34" s="23">
+      <c r="P34" s="20">
         <v>501.24</v>
       </c>
-      <c r="Q34" s="23">
+      <c r="Q34" s="20">
         <v>533.54</v>
       </c>
-      <c r="R34" s="23"/>
+      <c r="R34" s="20"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="27">
+      <c r="A35" s="23">
         <v>0.2</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="20">
         <v>90.64</v>
       </c>
-      <c r="C35" s="23">
+      <c r="C35" s="20">
         <v>-463.5</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="20">
         <v>431.99</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="20">
         <v>845.36</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="20">
         <v>635.46</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="20">
         <v>55.64</v>
       </c>
-      <c r="H35" s="23">
+      <c r="H35" s="20">
         <v>76.650000000000006</v>
       </c>
-      <c r="I35" s="23"/>
-      <c r="J35" s="27">
+      <c r="I35" s="20"/>
+      <c r="J35" s="23">
         <v>0.2</v>
       </c>
-      <c r="K35" s="23">
+      <c r="K35" s="20">
         <v>293.68</v>
       </c>
-      <c r="L35" s="23">
+      <c r="L35" s="20">
         <v>-269.83</v>
       </c>
-      <c r="M35" s="23">
+      <c r="M35" s="20">
         <v>161.91</v>
       </c>
-      <c r="N35" s="23">
+      <c r="N35" s="20">
         <v>1064.54</v>
       </c>
-      <c r="O35" s="23">
+      <c r="O35" s="20">
         <v>555.48</v>
       </c>
-      <c r="P35" s="23">
+      <c r="P35" s="20">
         <v>425.47</v>
       </c>
-      <c r="Q35" s="23">
+      <c r="Q35" s="20">
         <v>554.84</v>
       </c>
-      <c r="R35" s="23"/>
+      <c r="R35" s="20"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="27">
+      <c r="A36" s="23">
         <v>0.25</v>
       </c>
-      <c r="B36" s="23">
+      <c r="B36" s="20">
         <v>110.5</v>
       </c>
-      <c r="C36" s="23">
+      <c r="C36" s="20">
         <v>-287.86</v>
       </c>
-      <c r="D36" s="23">
+      <c r="D36" s="20">
         <v>365.91</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="20">
         <v>944.74</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="20">
         <v>658.86</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="20">
         <v>-139.5</v>
       </c>
-      <c r="H36" s="23">
+      <c r="H36" s="20">
         <v>77.95</v>
       </c>
-      <c r="I36" s="23"/>
-      <c r="J36" s="27">
+      <c r="I36" s="20"/>
+      <c r="J36" s="23">
         <v>0.25</v>
       </c>
-      <c r="K36" s="23">
+      <c r="K36" s="20">
         <v>420.61</v>
       </c>
-      <c r="L36" s="23">
+      <c r="L36" s="20">
         <v>-379.72</v>
       </c>
-      <c r="M36" s="23">
+      <c r="M36" s="20">
         <v>477.83</v>
       </c>
-      <c r="N36" s="23">
+      <c r="N36" s="20">
         <v>1258.52</v>
       </c>
-      <c r="O36" s="23">
+      <c r="O36" s="20">
         <v>635.13</v>
       </c>
-      <c r="P36" s="23">
+      <c r="P36" s="20">
         <v>243.29</v>
       </c>
-      <c r="Q36" s="23">
+      <c r="Q36" s="20">
         <v>477.61</v>
       </c>
-      <c r="R36" s="23"/>
+      <c r="R36" s="20"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="23"/>
-      <c r="Q37" s="23"/>
-      <c r="R37" s="23"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="24">
+      <c r="B38" s="21">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C38" s="24">
+      <c r="C38" s="21">
         <v>0.39930555555555558</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D38" s="21">
         <v>0.40277777777777801</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E38" s="21">
         <v>0.40625</v>
       </c>
-      <c r="F38" s="24">
+      <c r="F38" s="21">
         <v>0.40972222222222199</v>
       </c>
-      <c r="G38" s="24">
+      <c r="G38" s="21">
         <v>0.41319444444444497</v>
       </c>
-      <c r="H38" s="24">
+      <c r="H38" s="21">
         <v>0.41666666666666702</v>
       </c>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23" t="s">
+      <c r="I38" s="20"/>
+      <c r="J38" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="K38" s="24">
+      <c r="K38" s="21">
         <v>0.39583333333333331</v>
       </c>
-      <c r="L38" s="24">
+      <c r="L38" s="21">
         <v>0.39930555555555558</v>
       </c>
-      <c r="M38" s="24">
+      <c r="M38" s="21">
         <v>0.40277777777777801</v>
       </c>
-      <c r="N38" s="24">
+      <c r="N38" s="21">
         <v>0.40625</v>
       </c>
-      <c r="O38" s="24">
+      <c r="O38" s="21">
         <v>0.40972222222222199</v>
       </c>
-      <c r="P38" s="24">
+      <c r="P38" s="21">
         <v>0.41319444444444497</v>
       </c>
-      <c r="Q38" s="24">
+      <c r="Q38" s="21">
         <v>0.41666666666666702</v>
       </c>
-      <c r="R38" s="23"/>
+      <c r="R38" s="20"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="27">
+      <c r="A39" s="23">
         <v>0</v>
       </c>
-      <c r="B39" s="23">
+      <c r="B39" s="20">
         <f>SUM(B3, B10, B17, B24, B31)</f>
         <v>2858.86</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C39" s="20">
         <f t="shared" ref="C39:H39" si="0">SUM(C3, C10, C17, C24, C31)</f>
         <v>2345.08</v>
       </c>
-      <c r="D39" s="23">
+      <c r="D39" s="20">
         <f t="shared" si="0"/>
         <v>2245.42</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="20">
         <f t="shared" si="0"/>
         <v>2396.54</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="20">
         <f t="shared" si="0"/>
         <v>2321.48</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="20">
         <f t="shared" si="0"/>
         <v>3474.92</v>
       </c>
-      <c r="H39" s="23">
+      <c r="H39" s="20">
         <f t="shared" si="0"/>
         <v>2815.03</v>
       </c>
-      <c r="I39" s="29">
+      <c r="I39" s="24">
         <f>SUM(B39:H39)</f>
         <v>18457.330000000002</v>
       </c>
-      <c r="J39" s="27">
+      <c r="J39" s="23">
         <v>0</v>
       </c>
-      <c r="K39" s="23">
+      <c r="K39" s="20">
         <f>SUM(K3, K10, K17, K24, K31)</f>
         <v>3026.67</v>
       </c>
-      <c r="L39" s="23">
+      <c r="L39" s="20">
         <f t="shared" ref="L39:Q39" si="1">SUM(L3, L10, L17, L24, L31)</f>
         <v>3290.3899999999994</v>
       </c>
-      <c r="M39" s="23">
+      <c r="M39" s="20">
         <f t="shared" si="1"/>
         <v>3323.63</v>
       </c>
-      <c r="N39" s="23">
+      <c r="N39" s="20">
         <f t="shared" si="1"/>
         <v>2745.71</v>
       </c>
-      <c r="O39" s="23">
+      <c r="O39" s="20">
         <f t="shared" si="1"/>
         <v>3457.2400000000002</v>
       </c>
-      <c r="P39" s="23">
+      <c r="P39" s="20">
         <f t="shared" si="1"/>
         <v>5001.0099999999993</v>
       </c>
-      <c r="Q39" s="23">
+      <c r="Q39" s="20">
         <f t="shared" si="1"/>
         <v>2444.3599999999997</v>
       </c>
-      <c r="R39" s="29">
+      <c r="R39" s="24">
         <f>SUM(K39:Q39)</f>
         <v>23289.01</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="27">
+      <c r="A40" s="23">
         <v>0.05</v>
       </c>
-      <c r="B40" s="23">
+      <c r="B40" s="20">
         <f t="shared" ref="B40:H44" si="2">SUM(B4, B11, B18, B25, B32)</f>
         <v>3464.64</v>
       </c>
-      <c r="C40" s="23">
+      <c r="C40" s="20">
         <f t="shared" si="2"/>
         <v>1913.2400000000002</v>
       </c>
-      <c r="D40" s="23">
+      <c r="D40" s="20">
         <f t="shared" si="2"/>
         <v>2536.6800000000003</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="20">
         <f t="shared" si="2"/>
         <v>3367.1099999999997</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="20">
         <f t="shared" si="2"/>
         <v>2614</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G40" s="20">
         <f t="shared" si="2"/>
         <v>3937.3099999999995</v>
       </c>
-      <c r="H40" s="23">
+      <c r="H40" s="20">
         <f t="shared" si="2"/>
         <v>3102.46</v>
       </c>
-      <c r="I40" s="29">
+      <c r="I40" s="24">
         <f t="shared" ref="I40:I44" si="3">SUM(B40:H40)</f>
         <v>20935.439999999999</v>
       </c>
-      <c r="J40" s="27">
+      <c r="J40" s="23">
         <v>0.05</v>
       </c>
-      <c r="K40" s="23">
+      <c r="K40" s="20">
         <f t="shared" ref="K40:Q44" si="4">SUM(K4, K11, K18, K25, K32)</f>
         <v>3464.06</v>
       </c>
-      <c r="L40" s="23">
+      <c r="L40" s="20">
         <f t="shared" si="4"/>
         <v>2734.16</v>
       </c>
-      <c r="M40" s="23">
+      <c r="M40" s="20">
         <f t="shared" si="4"/>
         <v>3749.93</v>
       </c>
-      <c r="N40" s="23">
+      <c r="N40" s="20">
         <f t="shared" si="4"/>
         <v>3057.58</v>
       </c>
-      <c r="O40" s="23">
+      <c r="O40" s="20">
         <f t="shared" si="4"/>
         <v>3971.63</v>
       </c>
-      <c r="P40" s="23">
+      <c r="P40" s="20">
         <f t="shared" si="4"/>
         <v>3515.8599999999997</v>
       </c>
-      <c r="Q40" s="23">
+      <c r="Q40" s="20">
         <f t="shared" si="4"/>
         <v>2735.02</v>
       </c>
-      <c r="R40" s="29">
+      <c r="R40" s="24">
         <f t="shared" ref="R40:R44" si="5">SUM(K40:Q40)</f>
         <v>23228.240000000002</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="27">
+      <c r="A41" s="23">
         <v>0.1</v>
       </c>
-      <c r="B41" s="23">
+      <c r="B41" s="20">
         <f t="shared" si="2"/>
         <v>3223.5999999999995</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="20">
         <f t="shared" si="2"/>
         <v>1947.0800000000002</v>
       </c>
-      <c r="D41" s="23">
+      <c r="D41" s="20">
         <f t="shared" si="2"/>
         <v>3034.1</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E41" s="20">
         <f t="shared" si="2"/>
         <v>3083.64</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="20">
         <f t="shared" si="2"/>
         <v>2472.3900000000003</v>
       </c>
-      <c r="G41" s="23">
+      <c r="G41" s="20">
         <f t="shared" si="2"/>
         <v>3643.1200000000003</v>
       </c>
-      <c r="H41" s="23">
+      <c r="H41" s="20">
         <f t="shared" si="2"/>
         <v>3289.66</v>
       </c>
-      <c r="I41" s="29">
+      <c r="I41" s="24">
         <f t="shared" si="3"/>
         <v>20693.589999999997</v>
       </c>
-      <c r="J41" s="27">
+      <c r="J41" s="23">
         <v>0.1</v>
       </c>
-      <c r="K41" s="23">
+      <c r="K41" s="20">
         <f t="shared" si="4"/>
         <v>2490.85</v>
       </c>
-      <c r="L41" s="23">
+      <c r="L41" s="20">
         <f t="shared" si="4"/>
         <v>3801.7400000000002</v>
       </c>
-      <c r="M41" s="23">
+      <c r="M41" s="20">
         <f t="shared" si="4"/>
         <v>3452.99</v>
       </c>
-      <c r="N41" s="23">
+      <c r="N41" s="20">
         <f t="shared" si="4"/>
         <v>2508.56</v>
       </c>
-      <c r="O41" s="23">
+      <c r="O41" s="20">
         <f t="shared" si="4"/>
         <v>4436.9400000000005</v>
       </c>
-      <c r="P41" s="23">
+      <c r="P41" s="20">
         <f t="shared" si="4"/>
         <v>3244.87</v>
       </c>
-      <c r="Q41" s="23">
+      <c r="Q41" s="20">
         <f t="shared" si="4"/>
         <v>2770.2</v>
       </c>
-      <c r="R41" s="29">
+      <c r="R41" s="24">
         <f t="shared" si="5"/>
         <v>22706.15</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="27">
+      <c r="A42" s="23">
         <v>0.15</v>
       </c>
-      <c r="B42" s="23">
+      <c r="B42" s="20">
         <f t="shared" si="2"/>
         <v>3019.45</v>
       </c>
-      <c r="C42" s="23">
+      <c r="C42" s="20">
         <f t="shared" si="2"/>
         <v>2273.4399999999996</v>
       </c>
-      <c r="D42" s="23">
+      <c r="D42" s="20">
         <f t="shared" si="2"/>
         <v>2673.72</v>
       </c>
-      <c r="E42" s="23">
+      <c r="E42" s="20">
         <f t="shared" si="2"/>
         <v>2812.54</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="20">
         <f t="shared" si="2"/>
         <v>3624.91</v>
       </c>
-      <c r="G42" s="23">
+      <c r="G42" s="20">
         <f t="shared" si="2"/>
         <v>3725.6000000000004</v>
       </c>
-      <c r="H42" s="23">
+      <c r="H42" s="20">
         <f t="shared" si="2"/>
         <v>3816.37</v>
       </c>
-      <c r="I42" s="29">
+      <c r="I42" s="24">
         <f t="shared" si="3"/>
         <v>21946.029999999995</v>
       </c>
-      <c r="J42" s="27">
+      <c r="J42" s="23">
         <v>0.15</v>
       </c>
-      <c r="K42" s="23">
+      <c r="K42" s="20">
         <f t="shared" si="4"/>
         <v>2174.2999999999997</v>
       </c>
-      <c r="L42" s="23">
+      <c r="L42" s="20">
         <f t="shared" si="4"/>
         <v>3299.06</v>
       </c>
-      <c r="M42" s="23">
+      <c r="M42" s="20">
         <f t="shared" si="4"/>
         <v>2635.81</v>
       </c>
-      <c r="N42" s="23">
+      <c r="N42" s="20">
         <f t="shared" si="4"/>
         <v>2533.12</v>
       </c>
-      <c r="O42" s="23">
+      <c r="O42" s="20">
         <f t="shared" si="4"/>
         <v>4523.87</v>
       </c>
-      <c r="P42" s="23">
+      <c r="P42" s="20">
         <f t="shared" si="4"/>
         <v>2757.2699999999995</v>
       </c>
-      <c r="Q42" s="23">
+      <c r="Q42" s="20">
         <f t="shared" si="4"/>
         <v>3310.96</v>
       </c>
-      <c r="R42" s="29">
+      <c r="R42" s="24">
         <f t="shared" si="5"/>
         <v>21234.39</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="27">
+      <c r="A43" s="23">
         <v>0.2</v>
       </c>
-      <c r="B43" s="23">
+      <c r="B43" s="20">
         <f t="shared" si="2"/>
         <v>2616.5700000000002</v>
       </c>
-      <c r="C43" s="23">
+      <c r="C43" s="20">
         <f t="shared" si="2"/>
         <v>2470.7200000000003</v>
       </c>
-      <c r="D43" s="23">
+      <c r="D43" s="20">
         <f t="shared" si="2"/>
         <v>2914.2799999999997</v>
       </c>
-      <c r="E43" s="23">
+      <c r="E43" s="20">
         <f t="shared" si="2"/>
         <v>2699.26</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="20">
         <f>SUM(F7, F14, F21, F28, F35)</f>
         <v>4379.12</v>
       </c>
-      <c r="G43" s="23">
+      <c r="G43" s="20">
         <f t="shared" si="2"/>
         <v>4076.85</v>
       </c>
-      <c r="H43" s="23">
+      <c r="H43" s="20">
         <f t="shared" si="2"/>
         <v>3531.65</v>
       </c>
-      <c r="I43" s="29">
+      <c r="I43" s="24">
         <f t="shared" si="3"/>
         <v>22688.45</v>
       </c>
-      <c r="J43" s="27">
+      <c r="J43" s="23">
         <v>0.2</v>
       </c>
-      <c r="K43" s="23">
+      <c r="K43" s="20">
         <f t="shared" si="4"/>
         <v>2568.0699999999997</v>
       </c>
-      <c r="L43" s="23">
+      <c r="L43" s="20">
         <f t="shared" si="4"/>
         <v>4343.07</v>
       </c>
-      <c r="M43" s="23">
+      <c r="M43" s="20">
         <f t="shared" si="4"/>
         <v>2873.34</v>
       </c>
-      <c r="N43" s="23">
+      <c r="N43" s="20">
         <f t="shared" si="4"/>
         <v>1752.8600000000001</v>
       </c>
-      <c r="O43" s="23">
+      <c r="O43" s="20">
         <f t="shared" si="4"/>
         <v>4228.2100000000009</v>
       </c>
-      <c r="P43" s="23">
+      <c r="P43" s="20">
         <f t="shared" si="4"/>
         <v>3269.88</v>
       </c>
-      <c r="Q43" s="23">
+      <c r="Q43" s="20">
         <f t="shared" si="4"/>
         <v>3844.14</v>
       </c>
-      <c r="R43" s="29">
+      <c r="R43" s="24">
         <f t="shared" si="5"/>
         <v>22879.57</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="27">
+      <c r="A44" s="23">
         <v>0.25</v>
       </c>
-      <c r="B44" s="23">
+      <c r="B44" s="20">
         <f t="shared" si="2"/>
         <v>2909.14</v>
       </c>
-      <c r="C44" s="23">
+      <c r="C44" s="20">
         <f t="shared" si="2"/>
         <v>3093.29</v>
       </c>
-      <c r="D44" s="23">
+      <c r="D44" s="20">
         <f t="shared" si="2"/>
         <v>2343.31</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E44" s="20">
         <f t="shared" si="2"/>
         <v>2691.59</v>
       </c>
-      <c r="F44" s="23">
+      <c r="F44" s="20">
         <f t="shared" si="2"/>
         <v>3792.1400000000003</v>
       </c>
-      <c r="G44" s="23">
+      <c r="G44" s="20">
         <f t="shared" si="2"/>
         <v>4630.8999999999996</v>
       </c>
-      <c r="H44" s="23">
+      <c r="H44" s="20">
         <f t="shared" si="2"/>
         <v>3225.97</v>
       </c>
-      <c r="I44" s="29">
+      <c r="I44" s="24">
         <f t="shared" si="3"/>
         <v>22686.340000000004</v>
       </c>
-      <c r="J44" s="27">
+      <c r="J44" s="23">
         <v>0.25</v>
       </c>
-      <c r="K44" s="23">
+      <c r="K44" s="20">
         <f t="shared" si="4"/>
         <v>2182.67</v>
       </c>
-      <c r="L44" s="23">
+      <c r="L44" s="20">
         <f t="shared" si="4"/>
         <v>3741.8099999999995</v>
       </c>
-      <c r="M44" s="23">
+      <c r="M44" s="20">
         <f t="shared" si="4"/>
         <v>3417.8</v>
       </c>
-      <c r="N44" s="23">
+      <c r="N44" s="20">
         <f t="shared" si="4"/>
         <v>1841.19</v>
       </c>
-      <c r="O44" s="23">
+      <c r="O44" s="20">
         <f t="shared" si="4"/>
         <v>4373.6000000000004</v>
       </c>
-      <c r="P44" s="23">
+      <c r="P44" s="20">
         <f t="shared" si="4"/>
         <v>4584.41</v>
       </c>
-      <c r="Q44" s="23">
+      <c r="Q44" s="20">
         <f t="shared" si="4"/>
         <v>4242.6899999999996</v>
       </c>
-      <c r="R44" s="29">
+      <c r="R44" s="24">
         <f t="shared" si="5"/>
         <v>24384.17</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="29">
+      <c r="A45" s="20"/>
+      <c r="B45" s="24">
         <f>SUM(B39:B44)</f>
         <v>18092.259999999998</v>
       </c>
-      <c r="C45" s="29">
+      <c r="C45" s="24">
         <f t="shared" ref="C45:H45" si="6">SUM(C39:C44)</f>
         <v>14042.850000000002</v>
       </c>
-      <c r="D45" s="29">
+      <c r="D45" s="24">
         <f t="shared" si="6"/>
         <v>15747.51</v>
       </c>
-      <c r="E45" s="29">
+      <c r="E45" s="24">
         <f t="shared" si="6"/>
         <v>17050.68</v>
       </c>
-      <c r="F45" s="29">
+      <c r="F45" s="24">
         <f t="shared" si="6"/>
         <v>19204.039999999997</v>
       </c>
-      <c r="G45" s="29">
+      <c r="G45" s="24">
         <f t="shared" si="6"/>
         <v>23488.699999999997</v>
       </c>
-      <c r="H45" s="29">
+      <c r="H45" s="24">
         <f t="shared" si="6"/>
         <v>19781.140000000003</v>
       </c>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="29">
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="24">
         <f>SUM(K39:K44)</f>
         <v>15906.619999999999</v>
       </c>
-      <c r="L45" s="29">
+      <c r="L45" s="24">
         <f t="shared" ref="L45:Q45" si="7">SUM(L39:L44)</f>
         <v>21210.229999999996</v>
       </c>
-      <c r="M45" s="29">
+      <c r="M45" s="24">
         <f t="shared" si="7"/>
         <v>19453.5</v>
       </c>
-      <c r="N45" s="29">
+      <c r="N45" s="24">
         <f t="shared" si="7"/>
         <v>14439.020000000002</v>
       </c>
-      <c r="O45" s="29">
+      <c r="O45" s="24">
         <f t="shared" si="7"/>
         <v>24991.489999999998</v>
       </c>
-      <c r="P45" s="29">
+      <c r="P45" s="24">
         <f t="shared" si="7"/>
         <v>22373.3</v>
       </c>
-      <c r="Q45" s="29">
+      <c r="Q45" s="24">
         <f t="shared" si="7"/>
         <v>19347.37</v>
       </c>
-      <c r="R45" s="23"/>
+      <c r="R45" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -5671,4 +5735,727 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29760C84-902C-408B-B9BF-83DDDFE5C351}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31:L32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="9" width="15.7109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="23.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1">
+        <v>22</v>
+      </c>
+      <c r="F3" s="19">
+        <v>0.43</v>
+      </c>
+      <c r="G3" s="13">
+        <v>64.72</v>
+      </c>
+      <c r="H3" s="13">
+        <v>2849.84</v>
+      </c>
+      <c r="I3" s="13">
+        <v>7394</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1">
+        <v>26</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0.43</v>
+      </c>
+      <c r="G4" s="13">
+        <v>218.16</v>
+      </c>
+      <c r="H4" s="13">
+        <v>3234.56</v>
+      </c>
+      <c r="I4" s="13">
+        <v>6074.96</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1">
+        <v>48</v>
+      </c>
+      <c r="C5" s="1">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
+        <v>60</v>
+      </c>
+      <c r="E5" s="1">
+        <v>22</v>
+      </c>
+      <c r="F5" s="19">
+        <v>0.42</v>
+      </c>
+      <c r="G5" s="13">
+        <v>64.72</v>
+      </c>
+      <c r="H5" s="13">
+        <v>2785.84</v>
+      </c>
+      <c r="I5" s="13">
+        <v>6888.96</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1">
+        <v>58</v>
+      </c>
+      <c r="E6" s="1">
+        <v>22</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0.43</v>
+      </c>
+      <c r="G6" s="13">
+        <v>64.72</v>
+      </c>
+      <c r="H6" s="13">
+        <v>2817.84</v>
+      </c>
+      <c r="I6" s="13">
+        <v>7784.96</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1">
+        <v>58</v>
+      </c>
+      <c r="E7" s="1">
+        <v>22</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0.44</v>
+      </c>
+      <c r="G7" s="13">
+        <v>64.72</v>
+      </c>
+      <c r="H7" s="13">
+        <v>2961.84</v>
+      </c>
+      <c r="I7" s="13">
+        <v>7882.96</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1">
+        <v>58</v>
+      </c>
+      <c r="E8" s="1">
+        <v>22</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.44</v>
+      </c>
+      <c r="G8" s="13">
+        <v>64.72</v>
+      </c>
+      <c r="H8" s="13">
+        <v>2889.84</v>
+      </c>
+      <c r="I8" s="13">
+        <v>8122.96</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1">
+        <v>56</v>
+      </c>
+      <c r="E12" s="1">
+        <v>22</v>
+      </c>
+      <c r="F12" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="G12" s="13">
+        <v>758.16</v>
+      </c>
+      <c r="H12" s="13">
+        <v>1626.48</v>
+      </c>
+      <c r="I12" s="13">
+        <v>5180</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1">
+        <v>48</v>
+      </c>
+      <c r="C13" s="1">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1">
+        <v>56</v>
+      </c>
+      <c r="E13" s="1">
+        <v>26</v>
+      </c>
+      <c r="F13" s="19">
+        <v>0.42</v>
+      </c>
+      <c r="G13" s="13">
+        <v>1014.16</v>
+      </c>
+      <c r="H13" s="13">
+        <v>1946.48</v>
+      </c>
+      <c r="I13" s="13">
+        <v>5436</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1">
+        <v>22</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0.39</v>
+      </c>
+      <c r="G14" s="13">
+        <v>726.16</v>
+      </c>
+      <c r="H14" s="13">
+        <v>1594.8</v>
+      </c>
+      <c r="I14" s="13">
+        <v>4636</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1">
+        <v>48</v>
+      </c>
+      <c r="C15" s="1">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="G15" s="13">
+        <v>742.16</v>
+      </c>
+      <c r="H15" s="13">
+        <v>1610.8</v>
+      </c>
+      <c r="I15" s="13">
+        <v>5564</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1">
+        <v>22</v>
+      </c>
+      <c r="F16" s="19">
+        <v>0.42</v>
+      </c>
+      <c r="G16" s="13">
+        <v>822.16</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1690.8</v>
+      </c>
+      <c r="I16" s="13">
+        <v>6156</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1">
+        <v>58</v>
+      </c>
+      <c r="E17" s="1">
+        <v>22</v>
+      </c>
+      <c r="F17" s="19">
+        <v>0.42</v>
+      </c>
+      <c r="G17" s="13">
+        <v>782.16</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1650.8</v>
+      </c>
+      <c r="I17" s="13">
+        <v>6420</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1">
+        <v>56</v>
+      </c>
+      <c r="E21" s="1">
+        <v>22</v>
+      </c>
+      <c r="F21" s="19">
+        <v>0.39</v>
+      </c>
+      <c r="G21" s="13">
+        <v>1290.4000000000001</v>
+      </c>
+      <c r="H21" s="13">
+        <v>1775.44</v>
+      </c>
+      <c r="I21" s="13">
+        <v>4812</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="1">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1">
+        <v>26</v>
+      </c>
+      <c r="F22" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="G22" s="13">
+        <v>1566.16</v>
+      </c>
+      <c r="H22" s="13">
+        <v>2051.1999999999998</v>
+      </c>
+      <c r="I22" s="13">
+        <v>4284</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1">
+        <v>60</v>
+      </c>
+      <c r="E23" s="1">
+        <v>22</v>
+      </c>
+      <c r="F23" s="19">
+        <v>0.39</v>
+      </c>
+      <c r="G23" s="13">
+        <v>1182.1600000000001</v>
+      </c>
+      <c r="H23" s="13">
+        <v>1667.2</v>
+      </c>
+      <c r="I23" s="13">
+        <v>5020</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1">
+        <v>48</v>
+      </c>
+      <c r="C24" s="1">
+        <v>22</v>
+      </c>
+      <c r="D24" s="1">
+        <v>58</v>
+      </c>
+      <c r="E24" s="1">
+        <v>22</v>
+      </c>
+      <c r="F24" s="19">
+        <v>0.39</v>
+      </c>
+      <c r="G24" s="13">
+        <v>1214.1600000000001</v>
+      </c>
+      <c r="H24" s="13">
+        <v>1699.2</v>
+      </c>
+      <c r="I24" s="13">
+        <v>5244</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1">
+        <v>58</v>
+      </c>
+      <c r="E25" s="1">
+        <v>22</v>
+      </c>
+      <c r="F25" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="G25" s="13">
+        <v>1278.1600000000001</v>
+      </c>
+      <c r="H25" s="13">
+        <v>1763.2</v>
+      </c>
+      <c r="I25" s="13">
+        <v>5308</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1">
+        <v>48</v>
+      </c>
+      <c r="C26" s="1">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1">
+        <v>58</v>
+      </c>
+      <c r="E26" s="1">
+        <v>22</v>
+      </c>
+      <c r="F26" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="G26" s="13">
+        <v>1246.1600000000001</v>
+      </c>
+      <c r="H26" s="13">
+        <v>1731.2</v>
+      </c>
+      <c r="I26" s="13">
+        <v>5556</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1.41</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>